<commit_message>
Added one graph and fixed Columns
</commit_message>
<xml_diff>
--- a/lab3/starter/src/Lab 3.xlsx
+++ b/lab3/starter/src/Lab 3.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/d3goel/ECE-254-Working/ECE254/lab3/starter/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08B8388F-0A61-C14E-A5F2-16913F186340}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE32100-507B-7A4C-A746-01EEAE60479D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{A9489093-A665-8E4A-B427-9D92B8FD26ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$9:$E$15</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -101,6 +105,1100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Time of Processes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>N = 100 B = 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.48527199999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46931600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50485599999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.485126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53655600000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.479688</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58155199999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-7EAC-1E4E-9AB7-C994C6714C38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>N =100 B = 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$9:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.48297200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47009400000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49681199999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48800199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53491</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48503400000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57974999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-7EAC-1E4E-9AB7-C994C6714C38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>N = 398 B = 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$16:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.69977599999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80072600000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78047</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82555199999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85140800000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66488400000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81520999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-7EAC-1E4E-9AB7-C994C6714C38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1067394239"/>
+        <c:axId val="1067358559"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1067394239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067358559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1067358559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067394239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1930400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED028521-8C2F-2141-89EB-4D8C491B232A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D152215A-F1A3-A147-90E3-64B7B5470738}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,10 +1529,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -457,10 +1555,10 @@
         <v>0.48527199999999998</v>
       </c>
       <c r="F2">
+        <v>0.35925400000000002</v>
+      </c>
+      <c r="G2">
         <v>7.1053402564500004E-2</v>
-      </c>
-      <c r="G2">
-        <v>0.35925400000000002</v>
       </c>
       <c r="H2">
         <v>0.11417776</v>
@@ -483,10 +1581,10 @@
         <v>0.46931600000000001</v>
       </c>
       <c r="F3">
+        <v>0.296296</v>
+      </c>
+      <c r="G3">
         <v>3.8420204892699997E-2</v>
-      </c>
-      <c r="G3">
-        <v>0.296296</v>
       </c>
       <c r="H3">
         <v>3.0741830000000001E-2</v>
@@ -509,10 +1607,10 @@
         <v>0.50485599999999997</v>
       </c>
       <c r="F4">
+        <v>0.31779400000000002</v>
+      </c>
+      <c r="G4">
         <v>0.168967497656</v>
-      </c>
-      <c r="G4">
-        <v>0.31779400000000002</v>
       </c>
       <c r="H4">
         <v>3.2508519999999999E-2</v>
@@ -535,10 +1633,10 @@
         <v>0.485126</v>
       </c>
       <c r="F5">
+        <v>0.24940599999999999</v>
+      </c>
+      <c r="G5">
         <v>4.8230800573900001E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.24940599999999999</v>
       </c>
       <c r="H5">
         <v>3.081385E-2</v>
@@ -561,10 +1659,10 @@
         <v>0.53655600000000003</v>
       </c>
       <c r="F6">
+        <v>0.28795999999999999</v>
+      </c>
+      <c r="G6">
         <v>5.2840655408499998E-2</v>
-      </c>
-      <c r="G6">
-        <v>0.28795999999999999</v>
       </c>
       <c r="H6">
         <v>8.5592299999999996E-2</v>
@@ -587,10 +1685,10 @@
         <v>0.479688</v>
       </c>
       <c r="F7">
+        <v>0.29296</v>
+      </c>
+      <c r="G7">
         <v>4.0167034443699998E-2</v>
-      </c>
-      <c r="G7">
-        <v>0.29296</v>
       </c>
       <c r="H7">
         <v>7.4220469999999997E-2</v>
@@ -613,10 +1711,10 @@
         <v>0.58155199999999996</v>
       </c>
       <c r="F8">
+        <v>0.27039400000000002</v>
+      </c>
+      <c r="G8">
         <v>3.4656302399399999E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.27039400000000002</v>
       </c>
       <c r="H8">
         <v>0.11448563</v>
@@ -639,10 +1737,10 @@
         <v>0.48297200000000001</v>
       </c>
       <c r="F9">
+        <v>0.31931399999999999</v>
+      </c>
+      <c r="G9">
         <v>6.7576587780100006E-2</v>
-      </c>
-      <c r="G9">
-        <v>0.31931399999999999</v>
       </c>
       <c r="H9">
         <v>8.2378510000000002E-2</v>
@@ -665,10 +1763,10 @@
         <v>0.47009400000000001</v>
       </c>
       <c r="F10">
+        <v>0.32397199999999998</v>
+      </c>
+      <c r="G10">
         <v>3.9035588428999998E-2</v>
-      </c>
-      <c r="G10">
-        <v>0.32397199999999998</v>
       </c>
       <c r="H10">
         <v>6.8559919999999996E-2</v>
@@ -691,10 +1789,10 @@
         <v>0.49681199999999998</v>
       </c>
       <c r="F11">
+        <v>0.33989599999999998</v>
+      </c>
+      <c r="G11">
         <v>4.7661941378799998E-2</v>
-      </c>
-      <c r="G11">
-        <v>0.33989599999999998</v>
       </c>
       <c r="H11">
         <v>6.3461900000000002E-2</v>
@@ -717,10 +1815,10 @@
         <v>0.48800199999999999</v>
       </c>
       <c r="F12">
+        <v>0.29674</v>
+      </c>
+      <c r="G12">
         <v>4.7628205886800001E-2</v>
-      </c>
-      <c r="G12">
-        <v>0.29674</v>
       </c>
       <c r="H12">
         <v>6.7975320000000006E-2</v>
@@ -743,10 +1841,10 @@
         <v>0.53491</v>
       </c>
       <c r="F13">
+        <v>0.30171199999999998</v>
+      </c>
+      <c r="G13">
         <v>5.2394521660199998E-2</v>
-      </c>
-      <c r="G13">
-        <v>0.30171199999999998</v>
       </c>
       <c r="H13">
         <v>6.8929539999999997E-2</v>
@@ -769,10 +1867,10 @@
         <v>0.48503400000000002</v>
       </c>
       <c r="F14">
+        <v>0.28117399999999998</v>
+      </c>
+      <c r="G14">
         <v>4.15710096582E-2</v>
-      </c>
-      <c r="G14">
-        <v>0.28117399999999998</v>
       </c>
       <c r="H14">
         <v>6.3235780000000005E-2</v>
@@ -795,10 +1893,10 @@
         <v>0.57974999999999999</v>
       </c>
       <c r="F15">
+        <v>0.30410999999999999</v>
+      </c>
+      <c r="G15">
         <v>3.3365124007000001E-2</v>
-      </c>
-      <c r="G15">
-        <v>0.30410999999999999</v>
       </c>
       <c r="H15">
         <v>0.29364383999999999</v>
@@ -821,10 +1919,10 @@
         <v>0.69977599999999995</v>
       </c>
       <c r="F16">
+        <v>0.52772200000000002</v>
+      </c>
+      <c r="G16">
         <v>7.5305762223099995E-2</v>
-      </c>
-      <c r="G16">
-        <v>0.52772200000000002</v>
       </c>
       <c r="H16">
         <v>6.0965470000000001E-2</v>
@@ -847,10 +1945,10 @@
         <v>0.80072600000000005</v>
       </c>
       <c r="F17">
+        <v>0.54853600000000002</v>
+      </c>
+      <c r="G17">
         <v>4.64974722324E-2</v>
-      </c>
-      <c r="G17">
-        <v>0.54853600000000002</v>
       </c>
       <c r="H17">
         <v>7.5772610000000004E-2</v>
@@ -873,10 +1971,10 @@
         <v>0.78047</v>
       </c>
       <c r="F18">
+        <v>0.66072799999999998</v>
+      </c>
+      <c r="G18">
         <v>4.3444459945999998E-2</v>
-      </c>
-      <c r="G18">
-        <v>0.66072799999999998</v>
       </c>
       <c r="H18">
         <v>6.3598100000000005E-2</v>
@@ -899,10 +1997,10 @@
         <v>0.82555199999999995</v>
       </c>
       <c r="F19">
+        <v>0.47683799999999998</v>
+      </c>
+      <c r="G19">
         <v>5.0743859687700003E-2</v>
-      </c>
-      <c r="G19">
-        <v>0.47683799999999998</v>
       </c>
       <c r="H19">
         <v>8.8950639999999997E-2</v>
@@ -925,10 +2023,10 @@
         <v>0.85140800000000005</v>
       </c>
       <c r="F20">
+        <v>0.58287999999999995</v>
+      </c>
+      <c r="G20">
         <v>4.9324248965399997E-2</v>
-      </c>
-      <c r="G20">
-        <v>0.58287999999999995</v>
       </c>
       <c r="H20">
         <v>6.5847020000000006E-2</v>
@@ -951,10 +2049,10 @@
         <v>0.66488400000000003</v>
       </c>
       <c r="F21">
+        <v>0.43586399999999997</v>
+      </c>
+      <c r="G21">
         <v>3.5085018797200003E-2</v>
-      </c>
-      <c r="G21">
-        <v>0.43586399999999997</v>
       </c>
       <c r="H21">
         <v>7.3660879999999998E-2</v>
@@ -977,10 +2075,10 @@
         <v>0.81520999999999999</v>
       </c>
       <c r="F22">
+        <v>0.41898800000000003</v>
+      </c>
+      <c r="G22">
         <v>4.84604364405E-2</v>
-      </c>
-      <c r="G22">
-        <v>0.41898800000000003</v>
       </c>
       <c r="H22">
         <v>0.17350999</v>
@@ -988,5 +2086,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>